<commit_message>
Working DevOps Agent Deployment
</commit_message>
<xml_diff>
--- a/aws_terraform/deployments/devops_agent/Terraform DevOpsAgent.xlsx
+++ b/aws_terraform/deployments/devops_agent/Terraform DevOpsAgent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfroggatt/Desktop/git/Personal/AWS-Automation/aws_terraform/deployments/devops_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D328165E-8EE3-ED43-AA35-8F91B3834BF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084741C-01F4-3B45-B902-BF950BF98617}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>VariableName</t>
   </si>
@@ -48,27 +48,18 @@
     <t>aws_access_key</t>
   </si>
   <si>
-    <t>********************</t>
-  </si>
-  <si>
     <t>The AWS Access Key</t>
   </si>
   <si>
     <t>aws_secret_key</t>
   </si>
   <si>
-    <t>****************************************</t>
-  </si>
-  <si>
     <t>The AWS Secret Key</t>
   </si>
   <si>
     <t>aws_region</t>
   </si>
   <si>
-    <t>us-east-2</t>
-  </si>
-  <si>
     <t>The AWS Region</t>
   </si>
   <si>
@@ -84,79 +75,94 @@
     <t>vpc_id</t>
   </si>
   <si>
+    <t>The vpc id to deploy the instances in to</t>
+  </si>
+  <si>
+    <t>corporate_ip</t>
+  </si>
+  <si>
+    <t>A single IP address to allow RDP / SSH connections</t>
+  </si>
+  <si>
+    <t>instance_key</t>
+  </si>
+  <si>
+    <t>The name of the EC2 instance key to use</t>
+  </si>
+  <si>
+    <t>environment_tag</t>
+  </si>
+  <si>
+    <t>An environment tag for the instances</t>
+  </si>
+  <si>
+    <t>owner_tag</t>
+  </si>
+  <si>
+    <t>An owner tag for the instances</t>
+  </si>
+  <si>
+    <t>devops_organisation</t>
+  </si>
+  <si>
+    <t>devops_pat</t>
+  </si>
+  <si>
+    <t>devops_pool_name</t>
+  </si>
+  <si>
+    <t>The Azure DevOps agent pool name</t>
+  </si>
+  <si>
+    <t>The Azure DevOps personal access token</t>
+  </si>
+  <si>
+    <t>The Azure DevOps organisation name</t>
+  </si>
+  <si>
+    <t>subnet_ids</t>
+  </si>
+  <si>
+    <t>Two subnet ids to deploy the instances in to</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>eu-west-2</t>
+  </si>
+  <si>
+    <t>212.139.37.214</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>xxxxxxxxxxxxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</t>
+  </si>
+  <si>
     <t>vpc-xxxxxxxx</t>
   </si>
   <si>
-    <t>The vpc id to deploy the instances in to</t>
-  </si>
-  <si>
-    <t>corporate_ip</t>
-  </si>
-  <si>
-    <t>86.7.1.174</t>
-  </si>
-  <si>
-    <t>A single IP address to allow RDP / SSH connections</t>
-  </si>
-  <si>
-    <t>instance_key</t>
-  </si>
-  <si>
-    <t>The name of the EC2 instance key to use</t>
-  </si>
-  <si>
-    <t>environment_tag</t>
-  </si>
-  <si>
-    <t>An environment tag for the instances</t>
-  </si>
-  <si>
-    <t>owner_tag</t>
-  </si>
-  <si>
-    <t>An owner tag for the instances</t>
-  </si>
-  <si>
-    <t>devops_organisation</t>
-  </si>
-  <si>
-    <t>devops_pat</t>
-  </si>
-  <si>
-    <t>devops_pool_name</t>
-  </si>
-  <si>
-    <t>cloudpea</t>
-  </si>
-  <si>
-    <t>****************************************************</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>Integration Team</t>
-  </si>
-  <si>
-    <t>The Azure DevOps agent pool name</t>
-  </si>
-  <si>
-    <t>The Azure DevOps personal access token</t>
-  </si>
-  <si>
-    <t>The Azure DevOps organisation name</t>
-  </si>
-  <si>
-    <t>subnet_ids</t>
-  </si>
-  <si>
     <t>subnet-xxxxxxxx, subnet-xxxxxxxx</t>
   </si>
   <si>
-    <t>Two subnet ids to deploy the instances in to</t>
-  </si>
-  <si>
-    <t>List</t>
+    <t>&lt;Key_Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Org_Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Personal_Access_Token&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Pool_Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Owner&gt;</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1055,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,187 +1085,189 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{38992879-B0A8-464B-BF2E-42CF927AF60B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{349CBF2E-84A1-1F40-8F56-387B92F0FC01}">
       <formula1>"t3.nano,t3.micro,t3.small,t3.medium,t3.large,t3.xlarge"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{B1D5C831-8ADA-8043-9FA3-799FEAFFF7DA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{C4922003-0938-0946-A2F5-F000AC04F334}">
       <formula1>"us-east-2,us-east-1,us-west-1,us-west-2,ap-south-1,ap-northeast-3,ap-northeast-2,ap-southeast-1,ap-southeast-2,ap-northeast-1,ca-central-1,cn-north-1,cn-northwest-1,eu-central-1,eu-west-1,eu-west-2,eu-west-3,eu-north-1,sa-east-1"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>